<commit_message>
[offers][fix] fix binance salary
</commit_message>
<xml_diff>
--- a/apps/portal/prisma/salaries.xlsx
+++ b/apps/portal/prisma/salaries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stuartlong/Desktop/tech-interview-handbook/apps/portal/prisma/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003F53E3-3C03-2E43-B264-5DA7EB7B3F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F786F8-165A-EE4E-A0C9-BFC06FECF33B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -28,12 +28,12 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="All" guid="{FF2CC13D-313E-4E5D-948E-15A6E3D40D82}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Shopee Fresh Grads" guid="{95B52AD4-CE9C-43B5-ADDC-C1B3B279BDF7}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 1" guid="{05BF6B27-78E1-41B6-89CC-B623511C44F1}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter for all" guid="{2C57CA31-A5F3-4298-AAC2-CF1BEC295330}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Internships" guid="{96159FB4-A41E-41F0-82FC-34B374954062}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Fresh Grad" guid="{4839B331-E2E3-46A1-91FC-3920C5B6BEA7}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Internships" guid="{96159FB4-A41E-41F0-82FC-34B374954062}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter for all" guid="{2C57CA31-A5F3-4298-AAC2-CF1BEC295330}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{05BF6B27-78E1-41B6-89CC-B623511C44F1}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Shopee Fresh Grads" guid="{95B52AD4-CE9C-43B5-ADDC-C1B3B279BDF7}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="All" guid="{FF2CC13D-313E-4E5D-948E-15A6E3D40D82}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -3640,11 +3640,11 @@
   </sheetPr>
   <dimension ref="A1:AM660"/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D539" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J136" sqref="J136"/>
+      <selection pane="bottomRight" activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5306,7 +5306,7 @@
       </c>
       <c r="E57" s="8">
         <f>K57*12</f>
-        <v>1620000</v>
+        <v>135000</v>
       </c>
       <c r="F57" s="4">
         <v>0</v>
@@ -5318,7 +5318,8 @@
         <v>135000</v>
       </c>
       <c r="K57" s="8">
-        <v>135000</v>
+        <f>135000/12</f>
+        <v>11250</v>
       </c>
       <c r="AI57" s="10"/>
       <c r="AJ57" s="4"/>
@@ -5329,7 +5330,7 @@
         <v>44565.850571967589</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C58" s="9" t="s">
         <v>533</v>
@@ -20128,12 +20129,15 @@
   </sheetData>
   <autoFilter ref="A1:J560" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <customSheetViews>
-    <customSheetView guid="{96159FB4-A41E-41F0-82FC-34B374954062}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{4839B331-E2E3-46A1-91FC-3920C5B6BEA7}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:P626" xr:uid="{CA2EC8C4-BA52-6B4C-B926-4D941BC6B51D}">
+      <autoFilter ref="A2:P626" xr:uid="{DC2E1E87-F9C4-3440-8CAF-F984BBE7EE67}">
         <filterColumn colId="1">
           <filters>
-            <filter val="Internship"/>
+            <filter val="Fresh Grad"/>
+            <filter val="International Graduate program"/>
+            <filter val="Junior (0 - 3 years)"/>
+            <filter val="Mid (4 - 7 years)"/>
             <filter val="Mid Career Switch"/>
             <filter val="Semi-mid"/>
             <filter val="Senior (8+ years)"/>
@@ -20142,17 +20146,13 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{2C57CA31-A5F3-4298-AAC2-CF1BEC295330}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{FF2CC13D-313E-4E5D-948E-15A6E3D40D82}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:P44" xr:uid="{BBBD77B6-26C6-0843-A09C-71591586ED0E}"/>
-    </customSheetView>
-    <customSheetView guid="{05BF6B27-78E1-41B6-89CC-B623511C44F1}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="E1:E661" xr:uid="{2C19D8B3-8E67-E647-B2DC-9B007B0F70BD}"/>
+      <autoFilter ref="A1:J607" xr:uid="{F9C6B767-5982-104C-B93B-29A8667E6B6E}"/>
     </customSheetView>
     <customSheetView guid="{95B52AD4-CE9C-43B5-ADDC-C1B3B279BDF7}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:P630" xr:uid="{A47F7C22-EF38-944E-A6A8-12FA13717666}">
+      <autoFilter ref="A2:P630" xr:uid="{CD893D80-50FB-7E4B-BA07-BAD66E1696AD}">
         <filterColumn colId="1">
           <filters blank="1">
             <filter val="Fresh Grad"/>
@@ -20225,19 +20225,20 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{FF2CC13D-313E-4E5D-948E-15A6E3D40D82}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{05BF6B27-78E1-41B6-89CC-B623511C44F1}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:J607" xr:uid="{AE103217-4C9B-BF4C-918C-8C5FA7D36643}"/>
+      <autoFilter ref="E1:E661" xr:uid="{B7D54B01-0F42-A24C-9FE1-76C63BDD74A7}"/>
     </customSheetView>
-    <customSheetView guid="{4839B331-E2E3-46A1-91FC-3920C5B6BEA7}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{2C57CA31-A5F3-4298-AAC2-CF1BEC295330}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:P626" xr:uid="{21943F3E-EC55-F642-A838-2D7454477DA6}">
+      <autoFilter ref="A2:P44" xr:uid="{DD7EE174-F2E5-4E46-ADA3-8AD9400D4D87}"/>
+    </customSheetView>
+    <customSheetView guid="{96159FB4-A41E-41F0-82FC-34B374954062}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A2:P626" xr:uid="{F9DA054C-A6C6-4A41-8614-4B6E6C5BC2CE}">
         <filterColumn colId="1">
           <filters>
-            <filter val="Fresh Grad"/>
-            <filter val="International Graduate program"/>
-            <filter val="Junior (0 - 3 years)"/>
-            <filter val="Mid (4 - 7 years)"/>
+            <filter val="Internship"/>
             <filter val="Mid Career Switch"/>
             <filter val="Semi-mid"/>
             <filter val="Senior (8+ years)"/>
@@ -20260,7 +20261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DF8B4BB-B53A-A242-BD3A-33501EA08D94}">
   <dimension ref="A1:I160"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
+    <sheetView zoomScale="104" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[offers][fix] update tiktok salary
</commit_message>
<xml_diff>
--- a/apps/portal/prisma/salaries.xlsx
+++ b/apps/portal/prisma/salaries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stuartlong/Desktop/tech-interview-handbook/apps/portal/prisma/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F786F8-165A-EE4E-A0C9-BFC06FECF33B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7BC2D6-19F4-4C49-9AF0-4FF3DA2B44F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3641,10 +3641,10 @@
   <dimension ref="A1:AM660"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D37" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D484" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B58" sqref="B58"/>
+      <selection pane="bottomRight" activeCell="H497" sqref="H497"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -17893,7 +17893,8 @@
         <v>25000</v>
       </c>
       <c r="H496" s="4">
-        <v>103</v>
+        <f>E496+F496+I496</f>
+        <v>124900</v>
       </c>
       <c r="I496" s="4">
         <f>K496*1.5</f>
@@ -20261,8 +20262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DF8B4BB-B53A-A242-BD3A-33501EA08D94}">
   <dimension ref="A1:I160"/>
   <sheetViews>
-    <sheetView zoomScale="104" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView topLeftCell="A122" zoomScale="104" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>